<commit_message>
refactor|Price_serg,Currencies|update price, course currencies
</commit_message>
<xml_diff>
--- a/prices_for_processing/price_shik/Склад - Лист1.xlsx
+++ b/prices_for_processing/price_shik/Склад - Лист1.xlsx
@@ -161,7 +161,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -169,6 +169,7 @@
     </font>
     <font>
       <color theme="0"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -189,12 +190,8 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <name val="Arial"/>
     </font>
     <font>
@@ -205,9 +202,6 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
-    </font>
-    <font>
-      <color theme="5"/>
     </font>
   </fonts>
   <fills count="5">
@@ -242,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -264,37 +258,34 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -306,10 +297,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -620,7 +608,7 @@
       <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="7">
         <v>599.0</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -628,30 +616,30 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="9">
         <v>61470.0</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>499.0</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="9">
         <v>61503.0</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <v>240.0</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -659,13 +647,13 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="15">
         <v>300.0</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -676,10 +664,10 @@
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="17">
         <v>381.28</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -687,13 +675,13 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="7">
         <v>223.0</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -721,7 +709,7 @@
       <c r="B13" s="9">
         <v>62612.0</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="18">
         <v>265.0</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -729,7 +717,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -743,13 +731,13 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="7">
         <v>250.0</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -757,13 +745,13 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="15">
         <v>390.0</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -788,10 +776,10 @@
       <c r="A18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="7">
         <v>135.01</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -799,13 +787,13 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="7">
         <v>78.3</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -813,13 +801,13 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="7">
         <v>18.46</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -830,7 +818,7 @@
       <c r="A21" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="16" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="4">
@@ -841,13 +829,13 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="17">
         <v>109.0</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -858,7 +846,7 @@
       <c r="A23" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="20" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="6">
@@ -872,10 +860,10 @@
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="7">
         <v>350.0</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -883,39 +871,39 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
     </row>
     <row r="38">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="42">
-      <c r="A42" s="21"/>
-      <c r="B42" s="16"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="15"/>
     </row>
     <row r="45">
       <c r="A45" s="2"/>
-      <c r="B45" s="10"/>
+      <c r="B45" s="7"/>
     </row>
     <row r="51">
-      <c r="A51" s="21"/>
-      <c r="B51" s="16"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="15"/>
     </row>
     <row r="52">
-      <c r="A52" s="24"/>
-      <c r="B52" s="25"/>
+      <c r="A52" s="22"/>
+      <c r="B52" s="23"/>
     </row>
     <row r="53">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
     </row>
     <row r="54">
-      <c r="A54" s="23"/>
-      <c r="B54" s="18"/>
+      <c r="A54" s="21"/>
+      <c r="B54" s="17"/>
     </row>
     <row r="55">
-      <c r="A55" s="17"/>
+      <c r="A55" s="16"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
create|toAdmin|creating an administrator role
</commit_message>
<xml_diff>
--- a/prices_for_processing/price_shik/Склад - Лист1.xlsx
+++ b/prices_for_processing/price_shik/Склад - Лист1.xlsx
@@ -161,14 +161,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="0"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -188,13 +191,14 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -208,6 +212,8 @@
     </font>
     <font>
       <color theme="5"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -242,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -264,39 +270,36 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
@@ -306,10 +309,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -535,12 +535,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="55.43"/>
-    <col customWidth="1" min="2" max="2" width="21.0"/>
-    <col customWidth="1" min="3" max="3" width="15.14"/>
-    <col customWidth="1" min="4" max="4" width="13.57"/>
+    <col customWidth="1" min="1" max="1" width="48.5"/>
+    <col customWidth="1" min="2" max="2" width="18.38"/>
+    <col customWidth="1" min="3" max="3" width="13.25"/>
+    <col customWidth="1" min="4" max="4" width="11.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -620,7 +620,7 @@
       <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="7">
         <v>599.0</v>
       </c>
       <c r="D6" s="5" t="s">
@@ -628,30 +628,30 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="9">
         <v>61470.0</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <v>499.0</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="9">
         <v>61503.0</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <v>240.0</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -659,13 +659,13 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="15">
         <v>300.0</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -676,10 +676,10 @@
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="17">
         <v>381.28</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -687,13 +687,13 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="7">
         <v>223.0</v>
       </c>
       <c r="D11" s="5" t="s">
@@ -711,7 +711,7 @@
         <v>182.4</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13">
@@ -721,7 +721,7 @@
       <c r="B13" s="9">
         <v>62612.0</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="18">
         <v>265.0</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -729,7 +729,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -743,13 +743,13 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="7">
         <v>250.0</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -757,13 +757,13 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="13" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="16">
+      <c r="C16" s="15">
         <v>390.0</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -788,10 +788,10 @@
       <c r="A18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="7">
         <v>135.01</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -799,13 +799,13 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="7">
         <v>78.3</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -813,13 +813,13 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="7">
         <v>18.46</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -830,24 +830,24 @@
       <c r="A21" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="16" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="4">
         <v>44.8</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="17">
         <v>109.0</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -858,7 +858,7 @@
       <c r="A23" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="20" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="6">
@@ -872,10 +872,10 @@
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="10">
+      <c r="C24" s="7">
         <v>350.0</v>
       </c>
       <c r="D24" s="5" t="s">
@@ -883,39 +883,39 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
     </row>
     <row r="38">
-      <c r="A38" s="10"/>
-      <c r="B38" s="10"/>
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
     </row>
     <row r="42">
-      <c r="A42" s="21"/>
-      <c r="B42" s="16"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="15"/>
     </row>
     <row r="45">
       <c r="A45" s="2"/>
-      <c r="B45" s="10"/>
+      <c r="B45" s="7"/>
     </row>
     <row r="51">
-      <c r="A51" s="21"/>
-      <c r="B51" s="16"/>
+      <c r="A51" s="13"/>
+      <c r="B51" s="15"/>
     </row>
     <row r="52">
-      <c r="A52" s="24"/>
-      <c r="B52" s="25"/>
+      <c r="A52" s="22"/>
+      <c r="B52" s="23"/>
     </row>
     <row r="53">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
     </row>
     <row r="54">
-      <c r="A54" s="23"/>
-      <c r="B54" s="18"/>
+      <c r="A54" s="21"/>
+      <c r="B54" s="17"/>
     </row>
     <row r="55">
-      <c r="A55" s="17"/>
+      <c r="A55" s="16"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>